<commit_message>
Fix some errors in the data
Proofread the data entry and fixed errors. Created a csv file for the trap locations
</commit_message>
<xml_diff>
--- a/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
+++ b/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4845" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{014101E1-735E-42CA-AD90-BBCCE04BC4F8}"/>
+  <xr:revisionPtr revIDLastSave="4861" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{440E94B0-66B6-4010-BB5D-182DF309964D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11317" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11320" uniqueCount="1109">
   <si>
     <t>center_tree_number</t>
   </si>
@@ -3222,9 +3222,6 @@
     <t>bitternut hickory</t>
   </si>
   <si>
-    <t>white or green</t>
-  </si>
-  <si>
     <t>black and green</t>
   </si>
   <si>
@@ -3370,6 +3367,9 @@
   </si>
   <si>
     <t>20.7 cm Tilia 1-stem: 2 of 3 stems are gone - also needs a tree tag</t>
+  </si>
+  <si>
+    <t>Epicormic sprouts are big</t>
   </si>
 </sst>
 </file>
@@ -3918,7 +3918,7 @@
         <v>499</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -4023,7 +4023,7 @@
         <v>447</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -4052,7 +4052,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -4096,7 +4096,7 @@
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -4112,7 +4112,7 @@
         <v>545</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -4125,7 +4125,7 @@
         <v>27</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -4159,7 +4159,7 @@
         <v>443</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -4167,7 +4167,7 @@
         <v>28</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="87" x14ac:dyDescent="0.35">
@@ -4221,7 +4221,7 @@
         <v>33</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -4229,7 +4229,7 @@
         <v>34</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -6527,7 +6527,7 @@
         <v>815</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="M45" t="s">
         <v>442</v>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="J89" s="5"/>
       <c r="K89" s="5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L89" s="5" t="s">
         <v>799</v>
@@ -8662,7 +8662,7 @@
       </c>
       <c r="J95" s="5"/>
       <c r="L95" s="5" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="M95" t="s">
         <v>442</v>
@@ -8704,7 +8704,7 @@
       </c>
       <c r="J96" s="5"/>
       <c r="L96" s="5" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="M96" t="s">
         <v>442</v>
@@ -8746,7 +8746,7 @@
       </c>
       <c r="J97" s="5"/>
       <c r="L97" s="5" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="M97" t="s">
         <v>442</v>
@@ -8788,7 +8788,7 @@
       </c>
       <c r="J98" s="5"/>
       <c r="L98" s="5" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="M98" t="s">
         <v>442</v>
@@ -9316,10 +9316,10 @@
         <v>471</v>
       </c>
       <c r="J112" s="5" t="s">
+        <v>1101</v>
+      </c>
+      <c r="L112" s="5" t="s">
         <v>1102</v>
-      </c>
-      <c r="L112" s="5" t="s">
-        <v>1103</v>
       </c>
       <c r="M112" t="s">
         <v>442</v>
@@ -9461,8 +9461,8 @@
   </sheetPr>
   <dimension ref="A1:N397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M276" sqref="M276"/>
     </sheetView>
   </sheetViews>
@@ -26585,8 +26585,8 @@
   <dimension ref="A1:L397"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L265" sqref="L265"/>
+      <pane ySplit="1" topLeftCell="A383" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A386" sqref="A386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -37717,7 +37717,7 @@
         <v>437</v>
       </c>
       <c r="C378" t="s">
-        <v>1059</v>
+        <v>475</v>
       </c>
       <c r="D378">
         <v>1</v>
@@ -37749,7 +37749,7 @@
         <v>439</v>
       </c>
       <c r="C379" t="s">
-        <v>1059</v>
+        <v>475</v>
       </c>
       <c r="D379">
         <v>1</v>
@@ -37813,7 +37813,7 @@
         <v>438</v>
       </c>
       <c r="C381" t="s">
-        <v>1059</v>
+        <v>444</v>
       </c>
       <c r="D381">
         <v>0</v>
@@ -37909,7 +37909,7 @@
         <v>440</v>
       </c>
       <c r="C384" t="s">
-        <v>1060</v>
+        <v>754</v>
       </c>
       <c r="D384">
         <v>5</v>
@@ -37921,7 +37921,7 @@
         <v>441</v>
       </c>
       <c r="G384" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H384" t="s">
         <v>441</v>
@@ -37930,7 +37930,7 @@
         <v>441</v>
       </c>
       <c r="J384">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385" spans="1:10" x14ac:dyDescent="0.35">
@@ -37941,7 +37941,7 @@
         <v>438</v>
       </c>
       <c r="C385" t="s">
-        <v>754</v>
+        <v>1059</v>
       </c>
       <c r="D385">
         <v>5</v>
@@ -37953,7 +37953,7 @@
         <v>441</v>
       </c>
       <c r="G385" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H385" t="s">
         <v>441</v>
@@ -37962,7 +37962,7 @@
         <v>441</v>
       </c>
       <c r="J385">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.35">
@@ -38362,9 +38362,9 @@
   </sheetPr>
   <dimension ref="A1:S476"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A462" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K474" sqref="K474"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A432" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F444" sqref="F444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54373,7 +54373,7 @@
         <v>493</v>
       </c>
       <c r="F356">
-        <v>7.4</v>
+        <v>7.9</v>
       </c>
       <c r="G356">
         <v>1</v>
@@ -54440,6 +54440,9 @@
       <c r="N357" s="6" t="s">
         <v>441</v>
       </c>
+      <c r="R357" s="6" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="358" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A358">
@@ -54604,6 +54607,9 @@
       <c r="N361" t="s">
         <v>441</v>
       </c>
+      <c r="R361" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="362" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A362">
@@ -54892,7 +54898,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A369">
         <v>72</v>
       </c>
@@ -54933,7 +54939,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A370">
         <v>72</v>
       </c>
@@ -54974,7 +54980,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A371">
         <v>72</v>
       </c>
@@ -55015,7 +55021,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A372">
         <v>72</v>
       </c>
@@ -55056,7 +55062,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A373">
         <v>72</v>
       </c>
@@ -55097,7 +55103,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A374">
         <v>72</v>
       </c>
@@ -55138,7 +55144,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A375">
         <v>72</v>
       </c>
@@ -55179,7 +55185,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A376">
         <v>72</v>
       </c>
@@ -55220,7 +55226,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A377">
         <v>72</v>
       </c>
@@ -55261,7 +55267,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A378">
         <v>72</v>
       </c>
@@ -55301,8 +55307,11 @@
       <c r="N378" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R378" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="379" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A379">
         <v>72</v>
       </c>
@@ -55343,7 +55352,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A380">
         <v>72</v>
       </c>
@@ -55384,7 +55393,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="381" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A381" s="6">
         <v>60</v>
       </c>
@@ -55425,7 +55434,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A382">
         <v>60</v>
       </c>
@@ -55466,7 +55475,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A383">
         <v>60</v>
       </c>
@@ -55507,7 +55516,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A384">
         <v>60</v>
       </c>
@@ -57010,7 +57019,7 @@
         <v>586</v>
       </c>
       <c r="E413" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F413">
         <v>3.4</v>
@@ -57234,10 +57243,10 @@
         <v>441</v>
       </c>
       <c r="Q417" s="6" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="R417" s="6" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="418" spans="1:19" x14ac:dyDescent="0.35">
@@ -57366,7 +57375,7 @@
         <v>441</v>
       </c>
       <c r="R420" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="421" spans="1:19" x14ac:dyDescent="0.35">
@@ -57451,7 +57460,7 @@
         <v>441</v>
       </c>
       <c r="R422" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="423" spans="1:19" x14ac:dyDescent="0.35">
@@ -57468,7 +57477,7 @@
         <v>493</v>
       </c>
       <c r="F423">
-        <v>6.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G423">
         <v>3</v>
@@ -57495,10 +57504,10 @@
         <v>441</v>
       </c>
       <c r="Q423" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="R423" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="424" spans="1:19" x14ac:dyDescent="0.35">
@@ -57627,10 +57636,10 @@
         <v>441</v>
       </c>
       <c r="Q426" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="R426" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="427" spans="1:19" x14ac:dyDescent="0.35">
@@ -57756,10 +57765,10 @@
         <v>441</v>
       </c>
       <c r="Q429" t="s">
+        <v>1067</v>
+      </c>
+      <c r="R429" t="s">
         <v>1068</v>
-      </c>
-      <c r="R429" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="430" spans="1:19" x14ac:dyDescent="0.35">
@@ -57862,7 +57871,7 @@
         <v>441</v>
       </c>
       <c r="R431" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="432" spans="1:19" x14ac:dyDescent="0.35">
@@ -57906,7 +57915,7 @@
         <v>441</v>
       </c>
       <c r="R432" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="433" spans="1:18" x14ac:dyDescent="0.35">
@@ -57953,7 +57962,7 @@
         <v>441</v>
       </c>
       <c r="Q433" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="434" spans="1:18" x14ac:dyDescent="0.35">
@@ -57997,7 +58006,7 @@
         <v>441</v>
       </c>
       <c r="Q434" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="435" spans="1:18" x14ac:dyDescent="0.35">
@@ -58082,7 +58091,7 @@
         <v>441</v>
       </c>
       <c r="R436" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="437" spans="1:18" x14ac:dyDescent="0.35">
@@ -58348,7 +58357,7 @@
         <v>493</v>
       </c>
       <c r="F443">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G443">
         <v>1</v>
@@ -59330,7 +59339,7 @@
         <v>441</v>
       </c>
       <c r="R466" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="467" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -59415,7 +59424,7 @@
         <v>441</v>
       </c>
       <c r="R468" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="469" spans="1:19" x14ac:dyDescent="0.35">
@@ -62198,7 +62207,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -62218,10 +62227,10 @@
         <v>764</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
@@ -62230,7 +62239,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -62263,7 +62272,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -62283,10 +62292,10 @@
         <v>764</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -62295,7 +62304,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -62345,10 +62354,10 @@
         <v>764</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -62404,10 +62413,10 @@
         <v>764</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
@@ -62463,10 +62472,10 @@
         <v>764</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
@@ -62522,10 +62531,10 @@
         <v>764</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -62534,7 +62543,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -62584,10 +62593,10 @@
         <v>764</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -62596,7 +62605,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -62629,7 +62638,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -62649,10 +62658,10 @@
         <v>764</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
@@ -62691,7 +62700,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -62714,7 +62723,7 @@
         <v>905</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
@@ -62753,7 +62762,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -62776,7 +62785,7 @@
         <v>905</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
@@ -62815,7 +62824,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -62838,7 +62847,7 @@
         <v>964</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H33" s="1">
         <v>0</v>
@@ -62897,7 +62906,7 @@
         <v>964</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
@@ -63047,7 +63056,7 @@
         <v>804</v>
       </c>
       <c r="F44" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -63064,13 +63073,13 @@
         <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F45" t="s">
         <v>905</v>
       </c>
       <c r="G45" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -63216,7 +63225,7 @@
         <v>804</v>
       </c>
       <c r="F53" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -63233,13 +63242,13 @@
         <v>14</v>
       </c>
       <c r="E54" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F54" t="s">
         <v>905</v>
       </c>
       <c r="G54" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -63385,7 +63394,7 @@
         <v>804</v>
       </c>
       <c r="F62" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -63402,13 +63411,13 @@
         <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F63" t="s">
         <v>905</v>
       </c>
       <c r="G63" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -63610,7 +63619,7 @@
         <v>804</v>
       </c>
       <c r="F7" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G7" t="s">
         <v>442</v>
@@ -63633,7 +63642,7 @@
         <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F8" t="s">
         <v>905</v>
@@ -63688,16 +63697,16 @@
         <v>909</v>
       </c>
       <c r="F10" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G10" t="s">
+        <v>442</v>
+      </c>
+      <c r="H10" t="s">
+        <v>441</v>
+      </c>
+      <c r="I10" t="s">
         <v>1076</v>
-      </c>
-      <c r="G10" t="s">
-        <v>442</v>
-      </c>
-      <c r="H10" t="s">
-        <v>441</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -63847,7 +63856,7 @@
         <v>804</v>
       </c>
       <c r="F17" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G17" t="s">
         <v>442</v>
@@ -63870,7 +63879,7 @@
         <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F18" t="s">
         <v>905</v>
@@ -63925,16 +63934,16 @@
         <v>909</v>
       </c>
       <c r="F20" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G20" t="s">
+        <v>442</v>
+      </c>
+      <c r="H20" t="s">
+        <v>441</v>
+      </c>
+      <c r="I20" t="s">
         <v>1076</v>
-      </c>
-      <c r="G20" t="s">
-        <v>442</v>
-      </c>
-      <c r="H20" t="s">
-        <v>441</v>
-      </c>
-      <c r="I20" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -64084,7 +64093,7 @@
         <v>804</v>
       </c>
       <c r="F27" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G27" t="s">
         <v>442</v>
@@ -64107,7 +64116,7 @@
         <v>103</v>
       </c>
       <c r="E28" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F28" t="s">
         <v>905</v>
@@ -64162,16 +64171,16 @@
         <v>909</v>
       </c>
       <c r="F30" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G30" t="s">
+        <v>442</v>
+      </c>
+      <c r="H30" t="s">
+        <v>441</v>
+      </c>
+      <c r="I30" t="s">
         <v>1076</v>
-      </c>
-      <c r="G30" t="s">
-        <v>442</v>
-      </c>
-      <c r="H30" t="s">
-        <v>441</v>
-      </c>
-      <c r="I30" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -64321,7 +64330,7 @@
         <v>804</v>
       </c>
       <c r="F37" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G37" t="s">
         <v>442</v>
@@ -64344,7 +64353,7 @@
         <v>104</v>
       </c>
       <c r="E38" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F38" t="s">
         <v>905</v>
@@ -64399,16 +64408,16 @@
         <v>909</v>
       </c>
       <c r="F40" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G40" t="s">
+        <v>442</v>
+      </c>
+      <c r="H40" t="s">
+        <v>441</v>
+      </c>
+      <c r="I40" t="s">
         <v>1076</v>
-      </c>
-      <c r="G40" t="s">
-        <v>442</v>
-      </c>
-      <c r="H40" t="s">
-        <v>441</v>
-      </c>
-      <c r="I40" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -64558,7 +64567,7 @@
         <v>804</v>
       </c>
       <c r="F47" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G47" t="s">
         <v>442</v>
@@ -64567,7 +64576,7 @@
         <v>441</v>
       </c>
       <c r="I47" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -64584,7 +64593,7 @@
         <v>105</v>
       </c>
       <c r="E48" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F48" t="s">
         <v>905</v>
@@ -64639,16 +64648,16 @@
         <v>909</v>
       </c>
       <c r="F50" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G50" t="s">
+        <v>442</v>
+      </c>
+      <c r="H50" t="s">
+        <v>441</v>
+      </c>
+      <c r="I50" t="s">
         <v>1076</v>
-      </c>
-      <c r="G50" t="s">
-        <v>442</v>
-      </c>
-      <c r="H50" t="s">
-        <v>441</v>
-      </c>
-      <c r="I50" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -64798,7 +64807,7 @@
         <v>804</v>
       </c>
       <c r="F57" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G57" t="s">
         <v>442</v>
@@ -64821,7 +64830,7 @@
         <v>106</v>
       </c>
       <c r="E58" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F58" t="s">
         <v>905</v>
@@ -64876,16 +64885,16 @@
         <v>909</v>
       </c>
       <c r="F60" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G60" t="s">
+        <v>442</v>
+      </c>
+      <c r="H60" t="s">
+        <v>441</v>
+      </c>
+      <c r="I60" t="s">
         <v>1076</v>
-      </c>
-      <c r="G60" t="s">
-        <v>442</v>
-      </c>
-      <c r="H60" t="s">
-        <v>441</v>
-      </c>
-      <c r="I60" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -65038,7 +65047,7 @@
         <v>804</v>
       </c>
       <c r="F67" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G67" t="s">
         <v>442</v>
@@ -65061,7 +65070,7 @@
         <v>107</v>
       </c>
       <c r="E68" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F68" t="s">
         <v>905</v>
@@ -65116,16 +65125,16 @@
         <v>909</v>
       </c>
       <c r="F70" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G70" t="s">
+        <v>442</v>
+      </c>
+      <c r="H70" t="s">
+        <v>441</v>
+      </c>
+      <c r="I70" t="s">
         <v>1076</v>
-      </c>
-      <c r="G70" t="s">
-        <v>442</v>
-      </c>
-      <c r="H70" t="s">
-        <v>441</v>
-      </c>
-      <c r="I70" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -65278,7 +65287,7 @@
         <v>804</v>
       </c>
       <c r="F77" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G77" t="s">
         <v>442</v>
@@ -65301,7 +65310,7 @@
         <v>108</v>
       </c>
       <c r="E78" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F78" t="s">
         <v>905</v>
@@ -65356,7 +65365,7 @@
         <v>909</v>
       </c>
       <c r="F80" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="G80" t="s">
         <v>442</v>
@@ -65365,7 +65374,7 @@
         <v>441</v>
       </c>
       <c r="I80" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -65521,7 +65530,7 @@
         <v>804</v>
       </c>
       <c r="F87" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G87" t="s">
         <v>442</v>
@@ -65544,7 +65553,7 @@
         <v>109</v>
       </c>
       <c r="E88" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F88" t="s">
         <v>905</v>
@@ -65599,16 +65608,16 @@
         <v>909</v>
       </c>
       <c r="F90" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G90" t="s">
+        <v>442</v>
+      </c>
+      <c r="H90" t="s">
+        <v>441</v>
+      </c>
+      <c r="I90" t="s">
         <v>1076</v>
-      </c>
-      <c r="G90" t="s">
-        <v>442</v>
-      </c>
-      <c r="H90" t="s">
-        <v>441</v>
-      </c>
-      <c r="I90" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -65761,7 +65770,7 @@
         <v>804</v>
       </c>
       <c r="F97" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G97" t="s">
         <v>442</v>
@@ -65784,7 +65793,7 @@
         <v>110</v>
       </c>
       <c r="E98" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F98" t="s">
         <v>905</v>
@@ -65839,16 +65848,16 @@
         <v>909</v>
       </c>
       <c r="F100" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G100" t="s">
+        <v>442</v>
+      </c>
+      <c r="H100" t="s">
+        <v>441</v>
+      </c>
+      <c r="I100" t="s">
         <v>1076</v>
-      </c>
-      <c r="G100" t="s">
-        <v>442</v>
-      </c>
-      <c r="H100" t="s">
-        <v>441</v>
-      </c>
-      <c r="I100" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -65998,7 +66007,7 @@
         <v>804</v>
       </c>
       <c r="F107" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G107" t="s">
         <v>442</v>
@@ -66021,7 +66030,7 @@
         <v>111</v>
       </c>
       <c r="E108" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F108" t="s">
         <v>905</v>
@@ -66076,16 +66085,16 @@
         <v>909</v>
       </c>
       <c r="F110" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G110" t="s">
+        <v>442</v>
+      </c>
+      <c r="H110" t="s">
+        <v>441</v>
+      </c>
+      <c r="I110" t="s">
         <v>1076</v>
-      </c>
-      <c r="G110" t="s">
-        <v>442</v>
-      </c>
-      <c r="H110" t="s">
-        <v>441</v>
-      </c>
-      <c r="I110" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -66244,7 +66253,7 @@
         <v>804</v>
       </c>
       <c r="F117" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G117" t="s">
         <v>442</v>
@@ -66267,7 +66276,7 @@
         <v>112</v>
       </c>
       <c r="E118" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F118" t="s">
         <v>905</v>
@@ -66322,16 +66331,16 @@
         <v>909</v>
       </c>
       <c r="F120" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G120" t="s">
+        <v>442</v>
+      </c>
+      <c r="H120" t="s">
+        <v>441</v>
+      </c>
+      <c r="I120" t="s">
         <v>1076</v>
-      </c>
-      <c r="G120" t="s">
-        <v>442</v>
-      </c>
-      <c r="H120" t="s">
-        <v>441</v>
-      </c>
-      <c r="I120" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -66481,7 +66490,7 @@
         <v>804</v>
       </c>
       <c r="F127" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G127" t="s">
         <v>442</v>
@@ -66504,7 +66513,7 @@
         <v>113</v>
       </c>
       <c r="E128" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F128" t="s">
         <v>905</v>
@@ -66559,16 +66568,16 @@
         <v>909</v>
       </c>
       <c r="F130" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G130" t="s">
+        <v>442</v>
+      </c>
+      <c r="H130" t="s">
+        <v>441</v>
+      </c>
+      <c r="I130" t="s">
         <v>1076</v>
-      </c>
-      <c r="G130" t="s">
-        <v>442</v>
-      </c>
-      <c r="H130" t="s">
-        <v>441</v>
-      </c>
-      <c r="I130" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="132" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -66718,7 +66727,7 @@
         <v>804</v>
       </c>
       <c r="F137" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G137" t="s">
         <v>442</v>
@@ -66741,7 +66750,7 @@
         <v>114</v>
       </c>
       <c r="E138" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F138" t="s">
         <v>905</v>
@@ -66796,16 +66805,16 @@
         <v>909</v>
       </c>
       <c r="F140" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G140" t="s">
+        <v>442</v>
+      </c>
+      <c r="H140" t="s">
+        <v>441</v>
+      </c>
+      <c r="I140" t="s">
         <v>1076</v>
-      </c>
-      <c r="G140" t="s">
-        <v>442</v>
-      </c>
-      <c r="H140" t="s">
-        <v>441</v>
-      </c>
-      <c r="I140" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="142" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -66955,7 +66964,7 @@
         <v>804</v>
       </c>
       <c r="F147" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G147" t="s">
         <v>442</v>
@@ -66978,7 +66987,7 @@
         <v>115</v>
       </c>
       <c r="E148" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F148" t="s">
         <v>905</v>
@@ -67033,16 +67042,16 @@
         <v>909</v>
       </c>
       <c r="F150" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G150" t="s">
+        <v>442</v>
+      </c>
+      <c r="H150" t="s">
+        <v>441</v>
+      </c>
+      <c r="I150" t="s">
         <v>1076</v>
-      </c>
-      <c r="G150" t="s">
-        <v>442</v>
-      </c>
-      <c r="H150" t="s">
-        <v>441</v>
-      </c>
-      <c r="I150" t="s">
-        <v>1077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Copy tagged ash info into correct column
At the beginning of summer I was writing the tree tag info in the notes column, but I needed this to be in the tree_tag_info column. Also wrote more data-checking code
</commit_message>
<xml_diff>
--- a/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
+++ b/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4865" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFA93ADF-72CB-4624-9CC4-D4683006F04F}"/>
+  <xr:revisionPtr revIDLastSave="4871" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{546D87C8-C112-4BA4-8F29-52F3C8833C79}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4542,8 +4542,8 @@
   <dimension ref="A1:O114"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9462,8 +9462,8 @@
   <dimension ref="A1:N397"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M276" sqref="M276"/>
+      <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D343" sqref="D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -26585,8 +26585,8 @@
   <dimension ref="A1:L397"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A383" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A386" sqref="A386"/>
+      <pane ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A330" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38363,8 +38363,8 @@
   <dimension ref="A1:S477"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E409" sqref="E409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40109,7 +40109,7 @@
         <v>0</v>
       </c>
       <c r="Q31" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="R31" t="s">
         <v>452</v>
@@ -40483,7 +40483,7 @@
         <v>0</v>
       </c>
       <c r="Q38" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="R38" t="s">
         <v>452</v>
@@ -40539,7 +40539,7 @@
         <v>0</v>
       </c>
       <c r="Q39" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
       <c r="R39" t="s">
         <v>453</v>
@@ -40595,7 +40595,7 @@
         <v>0</v>
       </c>
       <c r="Q40" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="R40" t="s">
         <v>452</v>
@@ -56702,7 +56702,7 @@
     </row>
     <row r="406" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A406">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B406" t="s">
         <v>444</v>

</xml_diff>

<commit_message>
Work on ash trees
I made some edits to the R script where I created dataframes to summarize occurence of big and small trees.

Secondly I made an excel file of JUST tagged ash trees that we found. I also loaded 2011 data into a new folder, so we can compare the tagged ash to what size they were back in 2011.
</commit_message>
<xml_diff>
--- a/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
+++ b/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4871" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{546D87C8-C112-4BA4-8F29-52F3C8833C79}"/>
+  <xr:revisionPtr revIDLastSave="4877" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71A6919D-5D46-4388-B683-A098E19B5CAD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -38363,8 +38363,8 @@
   <dimension ref="A1:S477"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E409" sqref="E409"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Transect-level summaries and writing csvs
The folder Cleaned_data has many csvs that contain seedling, sapling, and tree data that has already been wrangled.
</commit_message>
<xml_diff>
--- a/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
+++ b/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4877" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71A6919D-5D46-4388-B683-A098E19B5CAD}"/>
+  <xr:revisionPtr revIDLastSave="4916" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B0C0AC-565D-48D1-96D4-E8F3F1855096}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11338" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11376" uniqueCount="1110">
   <si>
     <t>center_tree_number</t>
   </si>
@@ -3370,6 +3370,9 @@
   </si>
   <si>
     <t>Epicormic sprouts are big</t>
+  </si>
+  <si>
+    <t>See row 75_south</t>
   </si>
 </sst>
 </file>
@@ -3821,7 +3824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D88F145-B9A5-4ED2-BA4E-B069605466DD}">
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
@@ -4541,9 +4544,9 @@
   </sheetPr>
   <dimension ref="A1:O114"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:O23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4771,8 +4774,15 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="M5" t="s">
+        <v>441</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
@@ -4847,6 +4857,15 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="L7" s="5"/>
+      <c r="M7" t="s">
+        <v>441</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
@@ -7132,6 +7151,15 @@
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
       <c r="L59" s="5"/>
+      <c r="M59" t="s">
+        <v>441</v>
+      </c>
+      <c r="N59" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="O59" s="5" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="60" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
@@ -7735,12 +7763,25 @@
       <c r="H73" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I73" s="5"/>
+      <c r="I73" s="5" t="s">
+        <v>695</v>
+      </c>
       <c r="J73" s="5"/>
       <c r="K73" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="L73" s="5"/>
+      <c r="L73" s="5" t="s">
+        <v>1109</v>
+      </c>
+      <c r="M73" t="s">
+        <v>442</v>
+      </c>
+      <c r="N73" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="O73" s="5" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="74" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
@@ -8560,6 +8601,15 @@
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
       <c r="L92" s="5"/>
+      <c r="M92" t="s">
+        <v>441</v>
+      </c>
+      <c r="N92" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="O92" s="5" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="93" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
@@ -8589,6 +8639,15 @@
       <c r="I93" s="5"/>
       <c r="J93" s="5"/>
       <c r="L93" s="5"/>
+      <c r="M93" t="s">
+        <v>441</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="O93" s="5" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="94" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
@@ -9005,6 +9064,15 @@
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
       <c r="L103" s="5"/>
+      <c r="M103" t="s">
+        <v>441</v>
+      </c>
+      <c r="N103" t="s">
+        <v>441</v>
+      </c>
+      <c r="O103" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="104" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
@@ -9034,6 +9102,15 @@
       <c r="I104" s="5"/>
       <c r="J104" s="5"/>
       <c r="L104" s="5"/>
+      <c r="M104" t="s">
+        <v>441</v>
+      </c>
+      <c r="N104" t="s">
+        <v>441</v>
+      </c>
+      <c r="O104" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="105" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
@@ -9063,6 +9140,15 @@
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
       <c r="L105" s="5"/>
+      <c r="M105" t="s">
+        <v>441</v>
+      </c>
+      <c r="N105" t="s">
+        <v>441</v>
+      </c>
+      <c r="O105" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="106" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
@@ -9092,6 +9178,15 @@
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
       <c r="L106" s="5"/>
+      <c r="M106" t="s">
+        <v>441</v>
+      </c>
+      <c r="N106" t="s">
+        <v>441</v>
+      </c>
+      <c r="O106" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="107" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
@@ -9121,6 +9216,15 @@
       <c r="I107" s="5"/>
       <c r="J107" s="5"/>
       <c r="L107" s="5"/>
+      <c r="M107" t="s">
+        <v>441</v>
+      </c>
+      <c r="N107" t="s">
+        <v>441</v>
+      </c>
+      <c r="O107" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="108" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
@@ -9150,6 +9254,15 @@
       <c r="I108" s="5"/>
       <c r="J108" s="5"/>
       <c r="L108" s="5"/>
+      <c r="M108" t="s">
+        <v>441</v>
+      </c>
+      <c r="N108" t="s">
+        <v>441</v>
+      </c>
+      <c r="O108" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="109" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
@@ -38362,7 +38475,7 @@
   </sheetPr>
   <dimension ref="A1:S477"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>

</xml_diff>

<commit_message>
Mostly make graphs for grant proposal
</commit_message>
<xml_diff>
--- a/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
+++ b/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5288" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01B87D4C-E533-4FE7-846B-7E63311E8329}"/>
+  <xr:revisionPtr revIDLastSave="5291" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE98A1F4-D8F4-4A6C-A8F9-7B0691E38A7F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -3512,18 +3512,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -3848,7 +3843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D88F145-B9A5-4ED2-BA4E-B069605466DD}">
   <dimension ref="A1:B119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A108" workbookViewId="0">
       <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
@@ -9565,21 +9560,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M1:O1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O1048576">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="n">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="n">
       <formula>NOT(ISERROR(SEARCH("n",M2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",M2)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -38507,32 +38502,32 @@
   </sheetPr>
   <dimension ref="A1:T477"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.90625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1796875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="6" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.90625" customWidth="1"/>
+    <col min="2" max="2" width="4.1796875" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" customWidth="1"/>
-    <col min="6" max="6" width="5.453125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.453125" customWidth="1"/>
     <col min="7" max="7" width="4.54296875" customWidth="1"/>
-    <col min="8" max="8" width="5.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="7.08984375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1796875" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" customWidth="1"/>
+    <col min="11" max="11" width="7.08984375" customWidth="1"/>
     <col min="12" max="12" width="7.54296875" customWidth="1"/>
     <col min="13" max="13" width="6.08984375" customWidth="1"/>
-    <col min="14" max="14" width="5.26953125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7265625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="4.81640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="22.26953125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="5.26953125" customWidth="1"/>
+    <col min="15" max="15" width="5.7265625" customWidth="1"/>
+    <col min="16" max="16" width="4.81640625" customWidth="1"/>
+    <col min="17" max="17" width="22.26953125" customWidth="1"/>
     <col min="18" max="18" width="29.26953125" customWidth="1"/>
-    <col min="19" max="19" width="4.08984375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="4.08984375" customWidth="1"/>
     <col min="20" max="20" width="12.08984375" customWidth="1"/>
     <col min="21" max="21" width="21.1796875" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Modelling signs and symptoms
</commit_message>
<xml_diff>
--- a/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
+++ b/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5499" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C9BA54-1A9F-49BB-9E89-5E82C75B72BF}"/>
+  <xr:revisionPtr revIDLastSave="5508" documentId="8_{E6A25E5A-660E-410D-80FD-02C42A3E01DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFD9704-F160-4BD2-8BCC-B242DA4C2CED}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12052" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12056" uniqueCount="1119">
   <si>
     <t>center_tree_number</t>
   </si>
@@ -3395,6 +3395,12 @@
   </si>
   <si>
     <t>green_white_pumpkin_ash_present_y_n</t>
+  </si>
+  <si>
+    <t>yes or no question: were black ash seedlings found?</t>
+  </si>
+  <si>
+    <t>yes or no question: were green, white, or pumpkin ash seedlings found?</t>
   </si>
 </sst>
 </file>
@@ -3847,10 +3853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D88F145-B9A5-4ED2-BA4E-B069605466DD}">
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4057,7 +4063,7 @@
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>544</v>
       </c>
@@ -4065,17 +4071,17 @@
         <v>543</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -4083,485 +4089,505 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="41" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="45" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>1095</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>1098</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1093</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>546</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>1099</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="57" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>548</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="65" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>1091</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>1091</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>1110</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>1114</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="7" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="7" t="s">
         <v>550</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>551</v>
+        <v>456</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>18</v>
+        <v>592</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>480</v>
+        <v>458</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>465</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>553</v>
+        <v>480</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>554</v>
+        <v>468</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>476</v>
+        <v>460</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>549</v>
+        <v>476</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>510</v>
+        <v>462</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>463</v>
+        <v>30</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>464</v>
+        <v>510</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>20</v>
+        <v>463</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>35</v>
+        <v>464</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
+    <row r="96" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
+    <row r="97" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="7" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="7" t="s">
         <v>603</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>458</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>590</v>
+        <v>458</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>605</v>
+        <v>457</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="1"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="7" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="7" t="s">
         <v>604</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>458</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>590</v>
+        <v>458</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>606</v>
+        <v>457</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>607</v>
+        <v>590</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
         <v>591</v>
       </c>
     </row>
@@ -26731,8 +26757,8 @@
   <dimension ref="A1:N397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A389" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D403" sqref="D403"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27692,7 +27718,7 @@
         <v>441</v>
       </c>
       <c r="L57">
-        <v>0.3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
mostly stuff with the center trees
</commit_message>
<xml_diff>
--- a/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
+++ b/Raw_data/EAB_Michigan_2024_raw_data_photos_removed.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/EAB_Michigan_2024_2025_github_folder/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2161" documentId="8_{81CA749C-CDAC-43F8-B952-603FF177FEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE81AD9-BCEF-47A9-86FB-98C20FE7C57A}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{626AAFD1-2228-4D45-8913-C858FE942786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{056E0C0D-899D-4948-B477-8D3D143F4079}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -4203,10 +4203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D88F145-B9A5-4ED2-BA4E-B069605466DD}">
-  <dimension ref="A1:D155"/>
+  <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4331,838 +4331,843 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>542</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
+    <row r="33" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="10" t="s">
         <v>767</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>1095</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-    </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>543</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>1092</v>
       </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>1113</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>1115</v>
-      </c>
-      <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>1114</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>572</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>1093</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="7" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>1096</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>1091</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>1090</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>1097</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>548</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>1089</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>1108</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>1112</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="1"/>
-    </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="7" t="s">
         <v>550</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>0</v>
+        <v>456</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>551</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>591</v>
+        <v>459</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>458</v>
+        <v>591</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>18</v>
+        <v>458</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>480</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>465</v>
+        <v>480</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>553</v>
+        <v>465</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>554</v>
+        <v>469</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>476</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>30</v>
+        <v>462</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>510</v>
+        <v>30</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>463</v>
+        <v>510</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>20</v>
+        <v>464</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="1"/>
-    </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="7" t="s">
+      <c r="A103" s="1"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="7" t="s">
         <v>602</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>0</v>
+        <v>456</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>589</v>
+        <v>457</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>604</v>
+        <v>589</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="1"/>
-    </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="7" t="s">
         <v>603</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>0</v>
+        <v>456</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>589</v>
+        <v>457</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>605</v>
+        <v>589</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="4" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="4" t="s">
         <v>1145</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>589</v>
+        <v>457</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>1146</v>
+        <v>589</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>1131</v>
+        <v>1141</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>1146</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>1147</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>1117</v>
+        <v>1139</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>1152</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>1153</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>1142</v>
+        <v>1127</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>1128</v>
+        <v>1142</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>1157</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>1158</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>1126</v>
+        <v>1130</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>1132</v>
+        <v>1126</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>1159</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" s="1" t="s">
         <v>1134</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B151" s="1" t="s">
         <v>1160</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A151" s="1" t="s">
+    <row r="152" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
         <v>1135</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B152" s="1" t="s">
         <v>1161</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" s="1" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A154" s="1" t="s">
+    <row r="155" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
         <v>1138</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B155" s="1" t="s">
         <v>1162</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="1" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
         <v>1140</v>
       </c>
     </row>
@@ -5179,13 +5184,13 @@
   <dimension ref="A1:R114"/>
   <sheetViews>
     <sheetView zoomScale="59" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K101" sqref="K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="3.90625" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.36328125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="7.90625" customWidth="1"/>
@@ -11173,8 +11178,8 @@
   <dimension ref="A1:N397"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -28297,7 +28302,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M59" sqref="M59"/>
+      <selection pane="bottomLeft" sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40671,8 +40676,8 @@
   <dimension ref="A1:T477"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R92" sqref="R92"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -67375,7 +67380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1355A8E9-7FA3-45C2-9B00-12AFB3AD361D}">
   <dimension ref="A1:AU136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>